<commit_message>
add new test case
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16755" windowHeight="2910"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16755" windowHeight="2910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>url</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>kamao90</t>
+  </si>
+  <si>
+    <t>validdata</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
@@ -510,12 +513,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="3:3">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>